<commit_message>
[FEAT] Archivo preparado para el parseo
</commit_message>
<xml_diff>
--- a/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goo1ga\Documents\TEC\EEPROM_review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barajas\Documents\bosch_eeprom\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5602FBB0-3246-48DD-827D-39C62FFF61F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="0" windowWidth="24270" windowHeight="11790"/>
+    <workbookView xWindow="15180" yWindow="0" windowWidth="24270" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <r>
       <t>Purpose of the list: Collect project specific modifications in E²PROM container</t>
@@ -152,12 +153,21 @@
 BB9976
 (only allowed in case of type=datablock,plain)</t>
   </si>
+  <si>
+    <t>Id_Config__Org</t>
+  </si>
+  <si>
+    <t>TestData_07__Metadata</t>
+  </si>
+  <si>
+    <t>TestData_11__Metadata</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -207,6 +217,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3D3B3C"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -552,7 +568,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -733,10 +749,11 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1022,7 +1039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1030,10 +1047,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="60.42578125" style="9" hidden="1" customWidth="1"/>
@@ -1356,7 +1373,9 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
+      <c r="A12" s="80" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="27"/>
@@ -1379,7 +1398,9 @@
       <c r="U12" s="40"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
+      <c r="A13" s="80" t="s">
+        <v>38</v>
+      </c>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="27"/>
@@ -1402,7 +1423,9 @@
       <c r="U13" s="40"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="A14" s="80" t="s">
+        <v>39</v>
+      </c>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="27"/>
@@ -8578,7 +8601,7 @@
       <c r="U334" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A11:U11"/>
+  <autoFilter ref="A11:U11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="A11:V11">
     <sortCondition ref="A11"/>
   </sortState>
@@ -8599,7 +8622,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O12:O108">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O12:O108" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"range,datablock"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8613,7 +8636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8623,7 +8646,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>

</xml_diff>

<commit_message>
[FEAT]Se agregaron los comentarios, falta por confirmar si se tomara en cuenta el metadata de los datablock-name
</commit_message>
<xml_diff>
--- a/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -1761,7 +1761,15 @@
         </is>
       </c>
       <c r="P24" s="28" t="n"/>
-      <c r="Q24" s="38" t="n"/>
+      <c r="Q24" s="38" t="inlineStr">
+        <is>
+          <t>description=- Component: DUMMY
+- REPROG info: use case REPROG must not be set (data must not be changed after reprogramming)!
+Sometimes the description is longer than two rows.
+Other times, there are more than three.
+In this case, it is one more than four. And could be more.</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">

</xml_diff>

<commit_message>
[FEAT]Se agregaron nombre de encargado y nombre del proyecto
</commit_message>
<xml_diff>
--- a/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -999,7 +999,11 @@
           <t>Project</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n"/>
+      <c r="B2" s="7" t="inlineStr">
+        <is>
+          <t>BB-No=0123456789</t>
+        </is>
+      </c>
       <c r="C2" s="13" t="n"/>
       <c r="D2" s="13" t="n"/>
       <c r="E2" s="13" t="n"/>
@@ -1076,7 +1080,11 @@
           <t>Responsible</t>
         </is>
       </c>
-      <c r="B5" s="8" t="n"/>
+      <c r="B5" s="8" t="inlineStr">
+        <is>
+          <t>Oscar Gonzalez</t>
+        </is>
+      </c>
       <c r="C5" s="18" t="n"/>
       <c r="D5" s="18" t="n"/>
       <c r="E5" s="18" t="n"/>

</xml_diff>

<commit_message>
[FEAT] Autoinstalar librerias. Falta probarlo con una computadora que no tenga python
</commit_message>
<xml_diff>
--- a/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -1432,21 +1432,18 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TestData_08</t>
+          <t>TestData_07</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12346</v>
-      </c>
-      <c r="C18" t="n">
-        <v>87</v>
-      </c>
-      <c r="E18" t="inlineStr">
+        <v>12345</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1458,198 +1455,92 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>HOLA</t>
-        </is>
-      </c>
-      <c r="P18" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>JULIO</t>
-        </is>
-      </c>
-      <c r="R18" t="n">
-        <v>8</v>
-      </c>
-      <c r="S18" t="n">
-        <v>5</v>
+          <t>description=- Component: Test
+- REPROG info: To be evaluated.</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TestData_09</t>
+          <t>TestData_08</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12347</v>
-      </c>
-      <c r="C19" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" t="inlineStr">
+        <v>12346</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M19" t="inlineStr">
         <is>
           <t>ee_range</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>BB96</t>
-        </is>
-      </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>ADIOS</t>
-        </is>
-      </c>
-      <c r="P19" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>RUBEN</t>
-        </is>
-      </c>
-      <c r="R19" t="n">
-        <v>7</v>
-      </c>
-      <c r="S19" t="n">
-        <v>3</v>
+          <t>description=- Component: TST Data
+- REPROG info: undefined</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TestData_10</t>
+          <t>TestData_09</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12348</v>
-      </c>
-      <c r="C20" t="n">
-        <v>9</v>
-      </c>
-      <c r="D20" t="inlineStr">
+        <v>12347</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M20" t="inlineStr">
         <is>
           <t>ee_range</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>BB75</t>
-        </is>
-      </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>:(</t>
-        </is>
-      </c>
-      <c r="P20" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>JULIO Y RUBEN</t>
-        </is>
-      </c>
-      <c r="R20" t="n">
-        <v>6</v>
-      </c>
-      <c r="S20" t="n">
-        <v>6</v>
+          <t>description=- Component: TST Data
+- REPROG info: tbd</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TestData_11</t>
+          <t>TestData_10</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>12349</v>
-      </c>
-      <c r="C21" t="n">
-        <v>5</v>
-      </c>
-      <c r="D21" t="inlineStr">
+        <v>12348</v>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>datablock</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>BB89</t>
-        </is>
-      </c>
-      <c r="P21" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>JEJ</t>
-        </is>
-      </c>
-      <c r="R21" t="n">
-        <v>5</v>
-      </c>
-      <c r="S21" t="n">
-        <v>9</v>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>description=- Component: TST
+- REPROG info: t.b.d</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1661,136 +1552,100 @@
       <c r="B22" t="n">
         <v>12349</v>
       </c>
-      <c r="C22" t="n">
-        <v>5</v>
-      </c>
-      <c r="D22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>datablock</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>BB89</t>
-        </is>
-      </c>
-      <c r="P22" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>JEJ</t>
-        </is>
-      </c>
-      <c r="R22" t="n">
-        <v>5</v>
-      </c>
-      <c r="S22" t="n">
-        <v>9</v>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>description=- Component: TST
+- REPROG info: use case REPROG must be set</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DUMMY_TestModuleCnt</t>
+          <t>TestData_11</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>31416</v>
-      </c>
-      <c r="I23" t="inlineStr">
+        <v>12349</v>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>ee_erase</t>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>description=- Component: TST
+- REPROG info: use case REPROG must be set</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>DUMMY_TestModuleCnt</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>31416</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>ee_erase</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>ASDFClockTower</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B25" t="n">
         <v>111255</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="M25" t="inlineStr">
         <is>
           <t>ee_datablock</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
+      <c r="O25" t="inlineStr">
         <is>
           <t>description=- Component: ASDF
 - REPROG info: use case REPROG must not be set.
 - REPROG info: In certain cases there are two comments of this type.
 There are also strings up to 160 characters per row, only on description fields and usually is not only one row. Like this example but a little bit longer.</t>
         </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>TestData_07</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>123456</v>
-      </c>
-      <c r="C25" t="n">
-        <v>91</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>ee_range</t>
-        </is>
-      </c>
-      <c r="S25" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>